<commit_message>
testergebnisse nun alle auf private score acc
</commit_message>
<xml_diff>
--- a/neue_testergebnisse.xlsx
+++ b/neue_testergebnisse.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5928" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="6876" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
   <si>
     <t>Feature</t>
   </si>
@@ -88,9 +88,6 @@
     <t>gbm</t>
   </si>
   <si>
-    <t>0.518</t>
-  </si>
-  <si>
     <t>filtered average</t>
   </si>
   <si>
@@ -115,45 +112,27 @@
     <t>0.707</t>
   </si>
   <si>
-    <t>0.595</t>
-  </si>
-  <si>
     <t>0.582</t>
   </si>
   <si>
     <t>channel 39</t>
   </si>
   <si>
-    <t>0.609</t>
-  </si>
-  <si>
     <t>0.742</t>
   </si>
   <si>
-    <t>0.639</t>
-  </si>
-  <si>
     <t>svm</t>
   </si>
   <si>
     <t>0.598</t>
   </si>
   <si>
-    <t>0.647</t>
-  </si>
-  <si>
     <t>channel 46</t>
   </si>
   <si>
-    <t>0.697</t>
-  </si>
-  <si>
     <t>0.597</t>
   </si>
   <si>
-    <t>0.702</t>
-  </si>
-  <si>
     <t>channel 39, CP2</t>
   </si>
   <si>
@@ -163,9 +142,6 @@
     <t>0.601</t>
   </si>
   <si>
-    <t>0.678</t>
-  </si>
-  <si>
     <t>0.674</t>
   </si>
   <si>
@@ -187,9 +163,6 @@
     <t>5xdown, n200</t>
   </si>
   <si>
-    <t>0.623</t>
-  </si>
-  <si>
     <t>5xdown, n500</t>
   </si>
   <si>
@@ -202,16 +175,49 @@
     <t>0.489</t>
   </si>
   <si>
-    <t>0.636</t>
-  </si>
-  <si>
-    <t>0.630</t>
-  </si>
-  <si>
     <t>10xdown, alle</t>
   </si>
   <si>
-    <t>0.624</t>
+    <t>rf, entropy</t>
+  </si>
+  <si>
+    <t>0.670</t>
+  </si>
+  <si>
+    <t>0.672</t>
+  </si>
+  <si>
+    <t>0.606</t>
+  </si>
+  <si>
+    <t>0.628</t>
+  </si>
+  <si>
+    <t>0.626</t>
+  </si>
+  <si>
+    <t>0.653</t>
+  </si>
+  <si>
+    <t>0.644</t>
+  </si>
+  <si>
+    <t>0.990</t>
+  </si>
+  <si>
+    <t>0.587</t>
+  </si>
+  <si>
+    <t>0.576</t>
+  </si>
+  <si>
+    <t>0.604</t>
+  </si>
+  <si>
+    <t>0.564</t>
+  </si>
+  <si>
+    <t>0.690</t>
   </si>
 </sst>
 </file>
@@ -227,12 +233,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -275,19 +293,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -592,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:N56"/>
+  <dimension ref="B3:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,7 +650,7 @@
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -635,15 +659,15 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
@@ -651,11 +675,11 @@
       <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="J5" t="s">
         <v>5</v>
@@ -671,11 +695,11 @@
       <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>1496</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>29</v>
+      <c r="G6" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="K6" t="s">
         <v>7</v>
@@ -686,13 +710,13 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="1"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
@@ -700,17 +724,17 @@
       <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>33</v>
+      <c r="F8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
@@ -719,10 +743,10 @@
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
@@ -732,11 +756,11 @@
       <c r="E10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>1454</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>38</v>
+      <c r="G10" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
@@ -744,8 +768,8 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="1"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="7"/>
       <c r="K11" t="s">
         <v>15</v>
       </c>
@@ -755,7 +779,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>23</v>
@@ -763,10 +787,10 @@
       <c r="E12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>1812</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -780,8 +804,8 @@
       <c r="F13" s="3">
         <v>3378</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>26</v>
+      <c r="G13" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="H13" t="s">
         <v>20</v>
@@ -795,13 +819,13 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="1"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>23</v>
@@ -809,17 +833,17 @@
       <c r="E15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>1772</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>34</v>
+      <c r="G15" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>23</v>
@@ -827,11 +851,11 @@
       <c r="E16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>1840</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>36</v>
+      <c r="G16" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="J16" t="s">
         <v>10</v>
@@ -850,10 +874,10 @@
       <c r="F17" s="3">
         <v>3486</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="5"/>
+      <c r="G17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="4"/>
       <c r="K17" t="s">
         <v>12</v>
       </c>
@@ -863,8 +887,8 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="1"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="7"/>
       <c r="K18" t="s">
         <v>13</v>
       </c>
@@ -874,14 +898,14 @@
         <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="G19" s="7"/>
       <c r="K19" t="s">
         <v>14</v>
       </c>
@@ -892,14 +916,14 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
@@ -907,14 +931,14 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
@@ -922,11 +946,11 @@
       <c r="E23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F23" t="s">
-        <v>44</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>45</v>
+      <c r="F23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
@@ -936,17 +960,17 @@
       <c r="E24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="2">
         <v>1165</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>43</v>
+      <c r="G24" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>9</v>
@@ -954,11 +978,11 @@
       <c r="E25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F25" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" t="s">
-        <v>49</v>
+      <c r="F25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
@@ -968,129 +992,128 @@
       <c r="E26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="2">
         <v>1168</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>47</v>
+      <c r="G26" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F27" s="7">
+        <v>43</v>
+      </c>
+      <c r="F27" s="2">
         <v>1749</v>
       </c>
-      <c r="G27" t="s">
-        <v>52</v>
+      <c r="G27" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
-      <c r="C28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>23</v>
+      <c r="C28" s="1"/>
+      <c r="D28" t="s">
+        <v>54</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="7">
-        <v>1788</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N28" s="3"/>
+      <c r="F28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
-      <c r="C29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="7">
-        <v>1156</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N29" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1964</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="1"/>
-      <c r="N30" s="3"/>
+      <c r="G30" s="9"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="F31" s="2">
-        <v>1419</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H31" t="s">
-        <v>59</v>
-      </c>
+        <v>1788</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N31" s="3"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="C32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E32" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F32" s="2">
-        <v>13172</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F32" s="6">
+        <v>1156</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="N32" s="3"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="1"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7"/>
+      <c r="N33" s="3"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="E34" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1419</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
@@ -1098,13 +1121,13 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="F35" s="2">
-        <v>923597</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>65</v>
+        <v>13172</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
@@ -1113,79 +1136,83 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="1"/>
-      <c r="N36" s="3"/>
+      <c r="G36" s="7"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
+      <c r="E38" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F38" s="2">
+        <v>923597</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B39" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H39" t="s">
-        <v>55</v>
-      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="7"/>
+      <c r="N39" s="3"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+      <c r="F42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H42" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
@@ -1193,15 +1220,23 @@
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
+      <c r="D44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
@@ -1209,7 +1244,7 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
+      <c r="G45" s="7"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
@@ -1217,7 +1252,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
+      <c r="G46" s="7"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
@@ -1225,7 +1260,7 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
+      <c r="G47" s="7"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
@@ -1233,7 +1268,7 @@
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
+      <c r="G48" s="7"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
@@ -1241,7 +1276,7 @@
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
+      <c r="G49" s="7"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
@@ -1249,7 +1284,7 @@
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
+      <c r="G50" s="7"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
@@ -1257,7 +1292,7 @@
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
+      <c r="G51" s="7"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
@@ -1265,7 +1300,7 @@
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
+      <c r="G52" s="7"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
@@ -1273,7 +1308,7 @@
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
+      <c r="G53" s="7"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
@@ -1299,6 +1334,30 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>